<commit_message>
Added RMSE table for ADP
</commit_message>
<xml_diff>
--- a/RMSETable.xlsx
+++ b/RMSETable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvonckx\Documents\Repos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gjaniak\Documents\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
   <si>
     <t>Simulation</t>
   </si>
@@ -121,21 +121,21 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -454,203 +452,203 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>3.5024999999999999</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>5.8502000000000001</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>6.2819000000000003</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>20.462299999999999</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <v>4.2469000000000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="1">
         <v>2.8643999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>1.2349000000000001</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>5.5057999999999998</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>6.9206000000000003</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <v>21.070900000000002</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <v>1.3383</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="2">
         <v>1.7851999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>11</v>
+      <c r="C9" s="3">
+        <v>1.3067</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6.1990999999999996</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6.5789999999999997</v>
+      </c>
+      <c r="F9" s="3">
+        <v>21.192299999999999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.1877</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.6307</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
@@ -676,7 +674,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="7"/>
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -700,7 +698,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="7"/>
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -724,7 +722,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="7"/>
       <c r="B13" t="s">
         <v>12</v>
       </c>

</xml_diff>